<commit_message>
Update Dokumente nach Sprint Planning
</commit_message>
<xml_diff>
--- a/swe-iot/docs/PlanUndBurndown.xlsx
+++ b/swe-iot/docs/PlanUndBurndown.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1060" windowWidth="27760" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="1220" windowWidth="24540" windowHeight="15920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Story</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Melodien</t>
+  </si>
+  <si>
+    <t>SUMME</t>
+  </si>
+  <si>
+    <t>übrige Storypoints</t>
   </si>
 </sst>
 </file>
@@ -136,6 +142,964 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-AT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Storypoints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>übrige Storypoints</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2124158400"/>
+        <c:axId val="-2129288976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2124158400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2129288976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2129288976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2124158400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -412,7 +1376,7 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -434,8 +1398,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,8 +1424,12 @@
       <c r="H2">
         <v>8</v>
       </c>
+      <c r="I2">
+        <f>D14-H2</f>
+        <v>65</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
       </c>
@@ -471,8 +1442,18 @@
       <c r="F3">
         <v>2</v>
       </c>
+      <c r="G3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <f>I2-H3</f>
+        <v>57</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>3</v>
       </c>
@@ -482,8 +1463,11 @@
       <c r="D4">
         <v>5</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -496,8 +1480,11 @@
       <c r="D5">
         <v>8</v>
       </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -507,8 +1494,11 @@
       <c r="D6" s="1">
         <v>3</v>
       </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -518,8 +1508,11 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -532,8 +1525,11 @@
       <c r="D8" s="2">
         <v>20</v>
       </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
         <v>2</v>
@@ -545,7 +1541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2">
         <v>3</v>
@@ -557,7 +1553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -571,7 +1567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>2</v>
       </c>
@@ -580,9 +1576,19 @@
       </c>
       <c r="D12" s="2">
         <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <f>SUM(D2:D12)</f>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doku IT2 upgedatet nach Daily Scrum
</commit_message>
<xml_diff>
--- a/swe-iot/docs/PlanUndBurndown.xlsx
+++ b/swe-iot/docs/PlanUndBurndown.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1220" windowWidth="24540" windowHeight="15920" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="1220" windowWidth="27000" windowHeight="15920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Story</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Epic</t>
   </si>
@@ -41,9 +38,6 @@
     <t>erledigte Stories</t>
   </si>
   <si>
-    <t>Storypoints</t>
-  </si>
-  <si>
     <t>Kurzbezeichnung</t>
   </si>
   <si>
@@ -83,14 +77,23 @@
     <t>SUMME</t>
   </si>
   <si>
-    <t>übrige Storypoints</t>
+    <t>Storypoints pro Iteration</t>
+  </si>
+  <si>
+    <t>übrige Storypoints Plan</t>
+  </si>
+  <si>
+    <t>übrige Storypoints Ist</t>
+  </si>
+  <si>
+    <t>Story #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,6 +106,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -126,10 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -229,7 +241,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Storypoints</c:v>
+                  <c:v>Storypoints pro Iteration</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -282,7 +294,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>übrige Storypoints</c:v>
+                  <c:v>übrige Storypoints Ist</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -328,6 +340,79 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>übrige Storypoints Plan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="61000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -338,11 +423,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124158400"/>
-        <c:axId val="-2129288976"/>
+        <c:axId val="2130343712"/>
+        <c:axId val="2114933504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2124158400"/>
+        <c:axId val="2130343712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,7 +469,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129288976"/>
+        <c:crossAx val="2114933504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -392,7 +477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129288976"/>
+        <c:axId val="2114933504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +528,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124158400"/>
+        <c:crossAx val="2130343712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1071,16 +1156,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1365,52 +1450,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1428,13 +1522,18 @@
         <f>D14-H2</f>
         <v>65</v>
       </c>
+      <c r="J2">
+        <f>$D$14-SUM(D2)</f>
+        <v>65</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -1452,13 +1551,18 @@
         <f>I2-H3</f>
         <v>57</v>
       </c>
+      <c r="J3">
+        <f>$D$14-SUM(D2:D4)</f>
+        <v>57</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1466,16 +1570,20 @@
       <c r="F4">
         <v>3</v>
       </c>
+      <c r="J4">
+        <f>$D$14-SUM(D2:D5)</f>
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -1483,13 +1591,18 @@
       <c r="F5">
         <v>4</v>
       </c>
+      <c r="J5">
+        <f>$D$14-SUM(D2:D5)-SUM(D8)</f>
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -1497,13 +1610,18 @@
       <c r="F6">
         <v>5</v>
       </c>
+      <c r="J6">
+        <f>$D$14-SUM(D2:D5)-SUM(D8:D10)</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -1511,16 +1629,20 @@
       <c r="F7">
         <v>6</v>
       </c>
+      <c r="J7">
+        <f>$D$14-SUM(D2:D5)-SUM(D8:D11)</f>
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>3</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2">
         <v>20</v>
@@ -1528,61 +1650,69 @@
       <c r="F8">
         <v>7</v>
       </c>
+      <c r="J8">
+        <f>$D$14-SUM(D2:D5)-SUM(D8:D12)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
       <c r="B10" s="2">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>4</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
       <c r="B12" s="2">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3">
         <f>SUM(D2:D12)</f>
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Doku für Iteration 2
</commit_message>
<xml_diff>
--- a/swe-iot/docs/PlanUndBurndown.xlsx
+++ b/swe-iot/docs/PlanUndBurndown.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Epic</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Story #</t>
+  </si>
+  <si>
+    <t>2/3 nur teilweise</t>
   </si>
 </sst>
 </file>
@@ -277,9 +280,6 @@
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -333,7 +333,7 @@
                   <c:v>65.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.0</c:v>
+                  <c:v>65.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,15 +1541,12 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H3">
-        <v>8</v>
+      <c r="G3" t="s">
+        <v>21</v>
       </c>
       <c r="I3">
         <f>I2-H3</f>
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J3">
         <f>$D$14-SUM(D2:D4)</f>

</xml_diff>

<commit_message>
Update Doku nach Sprint 2
</commit_message>
<xml_diff>
--- a/swe-iot/docs/PlanUndBurndown.xlsx
+++ b/swe-iot/docs/PlanUndBurndown.xlsx
@@ -423,11 +423,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2130343712"/>
-        <c:axId val="2114933504"/>
+        <c:axId val="-2126470784"/>
+        <c:axId val="2081885440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2130343712"/>
+        <c:axId val="-2126470784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,7 +469,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2114933504"/>
+        <c:crossAx val="2081885440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -477,7 +477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114933504"/>
+        <c:axId val="2081885440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +528,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130343712"/>
+        <c:crossAx val="-2126470784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>

<commit_message>
update Color -> Problem bei behaviour Test
</commit_message>
<xml_diff>
--- a/swe-iot/docs/PlanUndBurndown.xlsx
+++ b/swe-iot/docs/PlanUndBurndown.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Epic</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>2/3 nur teilweise</t>
+  </si>
+  <si>
+    <t>1.2, 1.3, 2.1, 2.2</t>
   </si>
 </sst>
 </file>
@@ -280,6 +283,12 @@
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -334,6 +343,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,7 +1465,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1544,6 +1556,9 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="I3">
         <f>I2-H3</f>
         <v>65</v>
@@ -1566,6 +1581,17 @@
       </c>
       <c r="F4">
         <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <f>3+5+8+3</f>
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <f>I3-H4</f>
+        <v>46</v>
       </c>
       <c r="J4">
         <f>$D$14-SUM(D2:D5)</f>

</xml_diff>